<commit_message>
added document test classes fixed verify attributes method
</commit_message>
<xml_diff>
--- a/src/resources/data/Project.xlsx
+++ b/src/resources/data/Project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Separate Financial Statements\tests\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazen.Yousri\Downloads\playwright-sample-project-master\ECM_2\src\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE544EA1-741B-4AF8-B0FA-4170AF069F77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B182C777-6D5A-4DC0-BCC4-256AE102E51C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{32FD4DBE-343E-41BC-9339-A2040EB63184}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="54">
   <si>
     <t>Folder name</t>
   </si>
@@ -188,6 +188,15 @@
   </si>
   <si>
     <t>لا يسمح بإدخال تاريخ متقدم عن تاريخ اليوم</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>Not Approved</t>
+  </si>
+  <si>
+    <t>رقم الرزمة - النمار</t>
   </si>
 </sst>
 </file>
@@ -407,71 +416,6 @@
   <dxfs count="24">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -507,6 +451,23 @@
     </dxf>
     <dxf>
       <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -700,6 +661,54 @@
           <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -810,27 +819,27 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9110DB76-9602-4565-BAB2-BADB3455031C}" name="Folder name" dataDxfId="18"/>
     <tableColumn id="2" xr3:uid="{1990248A-4326-414A-ABF5-71E4B641E647}" name="Parent Folder" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{0C30F1D5-8CFB-463E-ACE6-9F03CB8B9E4D}" name="CanAdd" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{5AA35511-C994-4833-BB72-FE6BF87808B2}" name="Default" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{0C30F1D5-8CFB-463E-ACE6-9F03CB8B9E4D}" name="CanAdd" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{5AA35511-C994-4833-BB72-FE6BF87808B2}" name="Default" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{49DF0E64-46F8-4E17-85BF-377760A54903}" name="Table13" displayName="Table13" ref="A1:J29" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{49DF0E64-46F8-4E17-85BF-377760A54903}" name="Table13" displayName="Table13" ref="A1:J29" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="A1:J29" xr:uid="{B7B1CE8F-1EA5-40D9-BBDB-7FC6C9139EB5}"/>
   <tableColumns count="10">
-    <tableColumn id="2" xr3:uid="{B5211A4A-CC14-4E39-B5A3-D2DE29A9BC9C}" name="Document type" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{5813EE77-35A6-4D65-B05D-FB9CB62811E7}" name="Attribute name" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{778FAECF-2AD9-415D-A65E-3E0AE44C18DE}" name="Mandatory" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{5F1D1A2F-A965-4D74-9944-A3DCA8FD2361}" name="Attribute Type" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{25DEA50F-2269-4170-A508-B79EDC077711}" name="Max Length" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{340282AC-56C0-4FF3-B0DF-74CC1713E5EE}" name="List values" dataDxfId="6"/>
-    <tableColumn id="1" xr3:uid="{C1931490-E025-4105-A21C-C7DC0D6124C3}" name="Validation error" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{70361E95-A8BD-45CE-9C84-38F879C0E89A}" name="Future date" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{15BEBF61-3CD0-4E39-B60A-ADE27291BB3C}" name="Dependant" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{9A5B41C2-8644-4BF6-8F5C-F9D695432B03}" name="Default value" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{B5211A4A-CC14-4E39-B5A3-D2DE29A9BC9C}" name="Document type" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{5813EE77-35A6-4D65-B05D-FB9CB62811E7}" name="Attribute name" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{778FAECF-2AD9-415D-A65E-3E0AE44C18DE}" name="Mandatory" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{5F1D1A2F-A965-4D74-9944-A3DCA8FD2361}" name="Attribute Type" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{25DEA50F-2269-4170-A508-B79EDC077711}" name="Max Length" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{340282AC-56C0-4FF3-B0DF-74CC1713E5EE}" name="List values" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{C1931490-E025-4105-A21C-C7DC0D6124C3}" name="Validation error" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{70361E95-A8BD-45CE-9C84-38F879C0E89A}" name="Future date" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{15BEBF61-3CD0-4E39-B60A-ADE27291BB3C}" name="Dependant" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{9A5B41C2-8644-4BF6-8F5C-F9D695432B03}" name="Default value" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1135,15 +1144,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F8F9916-F296-4E41-9C5C-4C63E1135366}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="43.7265625" customWidth="1"/>
     <col min="2" max="2" width="42.26953125" customWidth="1"/>
-    <col min="3" max="4" width="8.7265625" style="25"/>
+    <col min="3" max="3" width="8.7265625" style="25"/>
+    <col min="4" max="4" width="17.81640625" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="46" customHeight="1" x14ac:dyDescent="0.35">
@@ -1209,8 +1219,8 @@
       <c r="D5" s="26"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="15">
-        <v>2024</v>
+      <c r="A6" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>26</v>
@@ -1380,7 +1390,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1567,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E716842-0CB7-4F20-A82A-BD6D4B710C48}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1661,7 +1671,9 @@
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="21"/>
+      <c r="J3" s="21" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
@@ -1877,7 +1889,9 @@
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="21"/>
+      <c r="J12" s="21" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -1997,14 +2011,16 @@
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="21"/>
+      <c r="J17" s="21" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>4</v>
@@ -2117,7 +2133,9 @@
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="21"/>
+      <c r="J22" s="21" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
@@ -2189,7 +2207,9 @@
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="21"/>
+      <c r="J25" s="21" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -2261,7 +2281,9 @@
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="21"/>
+      <c r="J28" s="21" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
@@ -2291,7 +2313,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C22 C24:C25 C30:C1048576 C27:C28" xr:uid="{B7826B1C-31AE-44CD-8E95-76E94E5D7300}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24:C25 C30:C1048576 C27:C28 C1:C22" xr:uid="{B7826B1C-31AE-44CD-8E95-76E94E5D7300}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{ECF814CF-4CA4-4827-B4BC-73CF744DBFA5}">

</xml_diff>

<commit_message>
Fixed entry template not waiting properly
</commit_message>
<xml_diff>
--- a/src/resources/data/Project.xlsx
+++ b/src/resources/data/Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazen.Yousri\Downloads\playwright-sample-project-master\ECM_2\src\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B182C777-6D5A-4DC0-BCC4-256AE102E51C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF99DF7-E1FA-4BF6-9991-082CC9498A07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{32FD4DBE-343E-41BC-9339-A2040EB63184}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="53">
   <si>
     <t>Folder name</t>
   </si>
@@ -194,9 +194,6 @@
   </si>
   <si>
     <t>Not Approved</t>
-  </si>
-  <si>
-    <t>رقم الرزمة - النمار</t>
   </si>
 </sst>
 </file>
@@ -1577,8 +1574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E716842-0CB7-4F20-A82A-BD6D4B710C48}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2020,7 +2017,7 @@
         <v>46</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
added document attributes tests
</commit_message>
<xml_diff>
--- a/src/resources/data/Project.xlsx
+++ b/src/resources/data/Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazen.Yousri\Downloads\playwright-sample-project-master\ECM_2\src\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9274A4CE-AAC6-4335-B480-1182FE996AEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946AD80E-0854-4A38-B910-9C385BCD9118}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{32FD4DBE-343E-41BC-9339-A2040EB63184}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="54">
   <si>
     <t>Folder name</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Not Approved</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -1574,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E716842-0CB7-4F20-A82A-BD6D4B710C48}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1632,19 +1635,21 @@
         <v>40</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="2">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="20"/>
+      <c r="J2" s="20" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -1654,7 +1659,7 @@
         <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>19</v>
@@ -1742,7 +1747,9 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="20"/>
+      <c r="J6" s="20" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -1766,7 +1773,9 @@
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="21"/>
+      <c r="J7" s="21" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -1862,7 +1871,9 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="20"/>
+      <c r="J11" s="20" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -1984,7 +1995,9 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="20"/>
+      <c r="J16" s="20" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -2106,7 +2119,9 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="20"/>
+      <c r="J21" s="20" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
@@ -2180,7 +2195,9 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="20"/>
+      <c r="J24" s="20" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
@@ -2254,7 +2271,9 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="20"/>
+      <c r="J27" s="20" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">

</xml_diff>

<commit_message>
changed list validation (wrong function, needs rework)
</commit_message>
<xml_diff>
--- a/src/resources/data/Project.xlsx
+++ b/src/resources/data/Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazen.Yousri\Downloads\playwright-sample-project-master\ECM_2\src\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946AD80E-0854-4A38-B910-9C385BCD9118}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B55EA24-E253-478C-AE43-662DF0DE6E8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{32FD4DBE-343E-41BC-9339-A2040EB63184}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="55">
   <si>
     <t>Folder name</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ,,دائن</t>
   </si>
 </sst>
 </file>
@@ -1578,7 +1581,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1816,7 +1819,7 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>

</xml_diff>

<commit_message>
Fixed List validation method (Normalized spaces) Added list validation test removed folder exist from attribut check method
</commit_message>
<xml_diff>
--- a/src/resources/data/Project.xlsx
+++ b/src/resources/data/Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazen.Yousri\Downloads\playwright-sample-project-master\ECM_2\src\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B55EA24-E253-478C-AE43-662DF0DE6E8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398736EC-0CB7-4F59-A841-A1C2815EBAD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{32FD4DBE-343E-41BC-9339-A2040EB63184}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="54">
   <si>
     <t>Folder name</t>
   </si>
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t>Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ,,دائن</t>
   </si>
 </sst>
 </file>
@@ -1580,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E716842-0CB7-4F20-A82A-BD6D4B710C48}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1694,7 +1691,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="3">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -1819,7 +1816,7 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>

</xml_diff>

<commit_message>
added verify addDoc page disappears after adding Added Security matrix test case
</commit_message>
<xml_diff>
--- a/src/resources/data/Project.xlsx
+++ b/src/resources/data/Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazen.Yousri\Downloads\playwright-sample-project-master\ECM_2\src\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398736EC-0CB7-4F59-A841-A1C2815EBAD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E28BCE4-FE47-4272-9170-8017B676EB2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{32FD4DBE-343E-41BC-9339-A2040EB63184}"/>
   </bookViews>
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E716842-0CB7-4F20-A82A-BD6D4B710C48}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1691,7 +1691,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="3">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>

</xml_diff>

<commit_message>
added new test ( check maker can view attr after approval )
</commit_message>
<xml_diff>
--- a/src/resources/data/Project.xlsx
+++ b/src/resources/data/Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazen.Yousri\Downloads\playwright-sample-project-master\ECM_2\src\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E28BCE4-FE47-4272-9170-8017B676EB2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF4DD6D-BDB3-4E22-8D01-D7E196438D39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{32FD4DBE-343E-41BC-9339-A2040EB63184}"/>
   </bookViews>
@@ -1390,7 +1390,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E716842-0CB7-4F20-A82A-BD6D4B710C48}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
arranged tests in order of execution Changed document cases before each
</commit_message>
<xml_diff>
--- a/src/resources/data/Project.xlsx
+++ b/src/resources/data/Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazen.Yousri\Downloads\playwright-sample-project-master\ECM_2\src\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12226EB0-1DB2-46A3-A42B-1F8F8D5EA3FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC5DFFC-41EB-42A8-9750-21C2DD80112B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{32FD4DBE-343E-41BC-9339-A2040EB63184}"/>
   </bookViews>
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E716842-0CB7-4F20-A82A-BD6D4B710C48}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>